<commit_message>
Update manual de usuario
</commit_message>
<xml_diff>
--- a/src/backend/the_only_excel.xlsx
+++ b/src/backend/the_only_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hlocal\TFG\src\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B1AC09-0F79-4570-8F64-7BB6664AC8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E911EEBE-91BC-488B-926E-E843223AC8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="100" windowWidth="14830" windowHeight="10240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPSS" sheetId="2" r:id="rId1"/>
@@ -1523,10 +1523,10 @@
   <dimension ref="A1:BP270"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AL252" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B268" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AX258" sqref="AX258"/>
+      <selection pane="bottomRight" activeCell="A271" sqref="A271:XFD271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.08203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>